<commit_message>
Error in corpus fixed
</commit_message>
<xml_diff>
--- a/Table 1 with authors.xlsx
+++ b/Table 1 with authors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Käyttäjä\PycharmProjects\HumanOrChatGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E0831C-BCDB-42C9-8CCF-271DD40D2961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B82DB3-70D9-4A8C-87F7-CA46E3DC5259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{6D8C0215-5990-4EED-8E53-4AB4317B62E6}"/>
   </bookViews>
@@ -708,15 +708,6 @@
   </si>
   <si>
     <t>Aleksis Kivi</t>
-  </si>
-  <si>
-    <t>Tuleen heitetty
-Idylli
-Muodon vaihdos
-Valtalaulu
-Musta mies
-Juomarit
-Excelsior</t>
   </si>
   <si>
     <t>L. Onerva</t>
@@ -2487,6 +2478,32 @@
   </si>
   <si>
     <t>Jonas Lie</t>
+  </si>
+  <si>
+    <t>Kuin käden vienon viileys
+saa kulmilleni mun,
+kuin häive, huntu, ilmestys
+maan oudon, salatun.
+Ah tunnenhan, ah tunnenhan
+ma, Sumuneiti, sun!
+Yön rimpi olen rauhaton,
+yön kuningatar sa,
+sun kruunus liljankukka on,
+ties niitun untuva.
+ Oi valtiatar varjon maan,
+mua raukkaa rakasta!
+On viittas unta viherää
+ja silmäsi kuin suo.
+Ma tuoksus tunnen, vaikk' en nää,
+sun suutas suuni juo.
+Ah, sallithan, ah sallithan
+mun jäädä yötä luo!
+Sun lempes yllein lankeaa
+kasteisin pisaroin.
+ Näin kyynelees mua armastaa
+valveeseen aamun koin.
+Yölintuna sun povellas
+ma kaikertelen, soin…</t>
   </si>
 </sst>
 </file>
@@ -2866,16 +2883,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D08C00CF-5093-4640-B914-08BEE42E51D1}">
   <dimension ref="A1:B160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="F96" sqref="F96"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="106.85546875" customWidth="1"/>
+    <col min="1" max="1" width="106.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2883,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2891,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2899,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2907,15 +2924,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="315" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -2923,23 +2940,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -2947,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2955,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -2963,15 +2980,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2979,23 +2996,23 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="290" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -3003,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>12</v>
       </c>
@@ -3011,7 +3028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -3019,7 +3036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -3027,7 +3044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -3035,7 +3052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
@@ -3043,7 +3060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -3051,7 +3068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -3059,7 +3076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>18</v>
       </c>
@@ -3067,23 +3084,23 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -3091,7 +3108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -3099,15 +3116,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>21</v>
       </c>
@@ -3115,7 +3132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -3123,7 +3140,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -3131,7 +3148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
@@ -3139,7 +3156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>28</v>
       </c>
@@ -3147,7 +3164,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
@@ -3155,7 +3172,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -3163,7 +3180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
@@ -3171,7 +3188,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -3179,7 +3196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
@@ -3187,7 +3204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>34</v>
       </c>
@@ -3195,23 +3212,23 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
@@ -3219,7 +3236,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
@@ -3227,7 +3244,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
@@ -3235,7 +3252,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="377" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>38</v>
       </c>
@@ -3243,15 +3260,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
@@ -3259,7 +3276,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
@@ -3267,7 +3284,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="203" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>40</v>
       </c>
@@ -3275,167 +3292,167 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="377" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="62" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="63" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B63" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="64" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="65" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="66" spans="1:2" ht="362.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B66" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B67" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" t="s">
+    <row r="68" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="69" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="70" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B61" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B63" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="375" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B66" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B68" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B69" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>42</v>
       </c>
@@ -3443,7 +3460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>44</v>
       </c>
@@ -3451,7 +3468,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>45</v>
       </c>
@@ -3459,55 +3476,55 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="116" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B74" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B75" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B76" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B77" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="87" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B78" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B79" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="405" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>47</v>
       </c>
@@ -3515,7 +3532,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>48</v>
       </c>
@@ -3523,636 +3540,636 @@
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" t="s">
         <v>50</v>
       </c>
-      <c r="B82" t="s">
+    </row>
+    <row r="83" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="B83" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B84" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B85" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="B86" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B86" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="B87" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B87" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="B88" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B88" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="B89" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B89" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="B90" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B90" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="B91" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" t="s">
         <v>65</v>
       </c>
-      <c r="B91" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    </row>
+    <row r="93" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B93" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="174" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B94" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="319" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B96" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B92" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="B98" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B99" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="145" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B100" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B101" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B102" t="s">
         <v>75</v>
       </c>
-      <c r="B93" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B94" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="315" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B95" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B96" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B97" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B98" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B99" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    </row>
+    <row r="103" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B103" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B100" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="315" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B101" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="B104" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B105" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B106" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A107" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B107" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+      <c r="A109" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" t="s">
         <v>85</v>
       </c>
-      <c r="B102" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B103" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    </row>
+    <row r="110" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A110" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B110" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="377" x14ac:dyDescent="0.35">
+      <c r="A111" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B104" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B105" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B106" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B107" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B108" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A112" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B112" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A113" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B113" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B114" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A115" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B115" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A116" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B116" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A117" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B117" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A118" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B118" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A119" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B119" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="319" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B120" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A121" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B110" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B111" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B112" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B113" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B114" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B115" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B116" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B117" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="B121" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="87" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B122" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="377" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B123" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A124" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B124" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A125" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B125" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A126" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B126" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A127" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B127" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+      <c r="A128" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B128" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+      <c r="A129" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B129" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A130" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B130" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A131" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B131" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
+      <c r="A132" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B118" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B119" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="B132" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A133" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B120" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B121" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B122" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B123" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B124" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B125" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B126" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B127" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B128" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B129" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B130" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="B133" t="s">
         <v>98</v>
       </c>
-      <c r="B131" t="s">
+    </row>
+    <row r="134" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A134" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B134" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A135" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B135" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+      <c r="A136" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" ht="405" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B132" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="345" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="B136" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+      <c r="A137" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B137" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A138" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B138" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+      <c r="A139" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B139" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="290" x14ac:dyDescent="0.35">
+      <c r="A140" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B140" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+      <c r="A141" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B141" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A142" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B133" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B134" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="B142" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A143" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B143" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A144" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B144" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A145" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B135" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B136" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="B145" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A146" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B146" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A147" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B147" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="116" x14ac:dyDescent="0.35">
+      <c r="A148" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B148" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A149" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B149" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A150" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B150" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="348" x14ac:dyDescent="0.35">
+      <c r="A151" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B151" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A152" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B152" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A153" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B153" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A154" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B154" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B155" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="203" x14ac:dyDescent="0.35">
+      <c r="A156" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B156" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A157" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B157" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="A158" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B158" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="232" x14ac:dyDescent="0.35">
+      <c r="A159" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B137" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B138" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B139" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B140" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B141" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B142" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B143" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B144" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B145" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B146" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B147" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B148" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B149" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B150" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B151" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B152" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B153" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B154" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B155" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B156" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B157" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B158" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
+      <c r="B159" t="s">
         <v>179</v>
       </c>
-      <c r="B159" t="s">
+    </row>
+    <row r="160" spans="1:2" ht="391.5" x14ac:dyDescent="0.35">
+      <c r="A160" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" ht="405" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
+      <c r="B160" t="s">
         <v>181</v>
-      </c>
-      <c r="B160" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>